<commit_message>
Might have clean subplot data for real this time - species info from 01.R is correct, monitoring events are correct, and SpeciesSeeded corrected based on each specific seed mix
</commit_message>
<xml_diff>
--- a/data/raw/03.1b_edited-species-seeded3_unk-corrected_subplot.xlsx
+++ b/data/raw/03.1b_edited-species-seeded3_unk-corrected_subplot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:40009_{09AA3EA2-7833-46D8-BF2B-61F162320472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEEB4C61-8831-4E71-8194-5F03483B21D9}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:40009_{09AA3EA2-7833-46D8-BF2B-61F162320472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBE97529-389F-45E5-83A3-84D5AF45252E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="202">
   <si>
     <t>Site</t>
   </si>
@@ -650,6 +650,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Unk bunchGrass #1.Pleasant</t>
   </si>
 </sst>
 </file>
@@ -1269,7 +1272,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> marked as not seeded.</a:t>
+            <a:t> are changed to be marked as not seeded.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1614,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="O77" sqref="O77"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3180,7 +3183,7 @@
         <v>60</v>
       </c>
       <c r="E49" t="s">
-        <v>60</v>
+        <v>201</v>
       </c>
       <c r="F49" t="s">
         <v>61</v>

</xml_diff>